<commit_message>
ADDED A NEW file
</commit_message>
<xml_diff>
--- a/datasheet1.xlsx
+++ b/datasheet1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python\RobotFramework1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python\RobotFrameworkRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>user1</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>pass5</t>
+  </si>
+  <si>
+    <t>ksallmx</t>
+  </si>
+  <si>
+    <t>bcnxd'lkj[</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,6 +445,21 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>